<commit_message>
Version 0.2 - Änderungen am Score-Script
</commit_message>
<xml_diff>
--- a/content/background_data_decision_tree.xlsx
+++ b/content/background_data_decision_tree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://skznet-my.sharepoint.com/personal/j_werner_skz_de/Documents/PlastIQ/Bearbeitung/AP3_Generische Modelle/Entwicklung Entscheidungsschema/02_Hintergrunddaten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="536" documentId="8_{03825F57-9271-4F19-AB31-225796C02C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95A585E3-DE1B-4FA1-A14B-69E033CD9C45}"/>
+  <xr:revisionPtr revIDLastSave="546" documentId="8_{03825F57-9271-4F19-AB31-225796C02C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B06D78FC-7D99-4334-8BC3-21700D70DEC3}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-2955" windowWidth="18240" windowHeight="28440" firstSheet="2" activeTab="5" xr2:uid="{9E0EC3E4-013A-49B8-ADD7-0C11DDD362E4}"/>
   </bookViews>
@@ -514,31 +514,7 @@
     <t xml:space="preserve">PS, </t>
   </si>
   <si>
-    <t>electric_DE_mix</t>
-  </si>
-  <si>
     <t>heat_DE_mix</t>
-  </si>
-  <si>
-    <t>electric_DE_wind</t>
-  </si>
-  <si>
-    <t>electric_DE_medium_voltage</t>
-  </si>
-  <si>
-    <t>electric_AT_medium_voltage</t>
-  </si>
-  <si>
-    <t>electric_CH_medium_voltage</t>
-  </si>
-  <si>
-    <t>electric_DE_green</t>
-  </si>
-  <si>
-    <t>electric_DE_water</t>
-  </si>
-  <si>
-    <t>electric_DE_solar</t>
   </si>
   <si>
     <t>heat_DE_natural_gas</t>
@@ -566,6 +542,30 @@
   </si>
   <si>
     <t>wastewater_DE_defaut</t>
+  </si>
+  <si>
+    <t>electricity_DE_medium_voltage</t>
+  </si>
+  <si>
+    <t>electricity_AT_medium_voltage</t>
+  </si>
+  <si>
+    <t>electricity_CH_medium_voltage</t>
+  </si>
+  <si>
+    <t>electricity_DE_green</t>
+  </si>
+  <si>
+    <t>electricity_DE_water</t>
+  </si>
+  <si>
+    <t>electricity_DE_wind</t>
+  </si>
+  <si>
+    <t>electricity_DE_solar</t>
+  </si>
+  <si>
+    <t>electricity_DE_mix</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1089,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16203,8 +16203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FB39F2-18C7-4C89-AECD-A2AD62B3166C}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17338,13 +17338,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B64" t="s">
         <v>120</v>
       </c>
       <c r="C64" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D64" s="2">
         <v>4.8232287999999998E-2</v>
@@ -17358,13 +17358,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B65" t="s">
         <v>121</v>
       </c>
       <c r="C65" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D65" s="2">
         <v>1.10681008</v>
@@ -17378,13 +17378,13 @@
     </row>
     <row r="66" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>149</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="D66" s="8">
         <v>0.3</v>
@@ -17393,172 +17393,172 @@
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D67" s="8">
-        <v>1</v>
-      </c>
-      <c r="E67" s="1" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>159</v>
+      </c>
+      <c r="B67" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" t="s">
+        <v>166</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.39970831275007851</v>
+      </c>
+      <c r="E67" t="s">
         <v>133</v>
+      </c>
+      <c r="F67" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B68" t="s">
+        <v>123</v>
+      </c>
+      <c r="C68" t="s">
         <v>167</v>
       </c>
-      <c r="B68" t="s">
-        <v>122</v>
-      </c>
-      <c r="C68" t="s">
-        <v>159</v>
-      </c>
       <c r="D68" s="2">
-        <v>0.39970831275007851</v>
+        <v>0.24423822562094591</v>
       </c>
       <c r="E68" t="s">
         <v>133</v>
       </c>
       <c r="F68" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B69" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C69" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D69" s="2">
-        <v>0.24423822562094591</v>
+        <v>0.11525018296731784</v>
       </c>
       <c r="E69" t="s">
         <v>133</v>
       </c>
       <c r="F69" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B70" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C70" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D70" s="2">
-        <v>0.11525018296731784</v>
+        <v>6.5184568658291961E-2</v>
       </c>
       <c r="E70" t="s">
         <v>133</v>
       </c>
       <c r="F70" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B71" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C71" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D71" s="2">
-        <v>6.5184568658291961E-2</v>
+        <v>6.0594767899999997E-3</v>
       </c>
       <c r="E71" t="s">
         <v>133</v>
       </c>
       <c r="F71" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B72" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C72" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D72" s="2">
-        <v>6.0594767899999997E-3</v>
+        <v>9.5242999999999994E-3</v>
       </c>
       <c r="E72" t="s">
         <v>133</v>
       </c>
       <c r="F72" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B73" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C73" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="D73" s="2">
-        <v>9.5242999999999994E-3</v>
+        <v>3.5394460000000003E-2</v>
       </c>
       <c r="E73" t="s">
         <v>133</v>
       </c>
       <c r="F73" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>167</v>
-      </c>
-      <c r="B74" t="s">
-        <v>128</v>
-      </c>
-      <c r="C74" t="s">
-        <v>164</v>
-      </c>
-      <c r="D74" s="2">
-        <v>3.5394460000000003E-2</v>
-      </c>
-      <c r="E74" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D74" s="8">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="F74" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B75" t="s">
         <v>129</v>
       </c>
       <c r="C75" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D75" s="2">
         <v>6.5247201979190747E-2</v>
@@ -17603,13 +17603,13 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C78" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Erweiterung der Sortierung um sort_sensorbased - Umarbeiten des df_result_sort mit Wechsel von Zeilen und Spalten
</commit_message>
<xml_diff>
--- a/content/background_data_decision_tree.xlsx
+++ b/content/background_data_decision_tree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://skznet-my.sharepoint.com/personal/j_werner_skz_de/Documents/PlastIQ/Bearbeitung/AP3_Generische Modelle/Entwicklung Entscheidungsschema/02_Hintergrunddaten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="659" documentId="8_{03825F57-9271-4F19-AB31-225796C02C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72B128A2-0F49-4640-ADDE-3808BC56B34F}"/>
+  <xr:revisionPtr revIDLastSave="692" documentId="8_{03825F57-9271-4F19-AB31-225796C02C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C6A3DC6-B4E7-46A9-AA6F-F7CB29D4FE4A}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-7665" windowWidth="29040" windowHeight="17640" xr2:uid="{9E0EC3E4-013A-49B8-ADD7-0C11DDD362E4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{9E0EC3E4-013A-49B8-ADD7-0C11DDD362E4}"/>
   </bookViews>
   <sheets>
     <sheet name="list_material" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="sort_eddycurrent" sheetId="3" r:id="rId3"/>
     <sheet name="sort_density" sheetId="4" r:id="rId4"/>
     <sheet name="sort_electrostatic" sheetId="5" r:id="rId5"/>
-    <sheet name="lca_calculation" sheetId="6" r:id="rId6"/>
+    <sheet name="sort_sensorbased" sheetId="7" r:id="rId6"/>
+    <sheet name="lca_calculation" sheetId="6" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="196">
   <si>
     <t>ABS</t>
   </si>
@@ -1156,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92B8105-A295-40FF-8933-641BD1D0C7D7}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -2223,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297DECE7-6377-4FBB-8C80-8873C3452F24}">
   <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AH34"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13077,8 +13078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838AB6B0-29DE-4DD8-811D-133F3C156F7B}">
   <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16691,6 +16692,3624 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D1A6FC-3E56-461B-B763-C2D2BC11EE1A}">
+  <dimension ref="A1:AH34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1:AH34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="9" t="str">
+        <f>A2</f>
+        <v>PE-LD</v>
+      </c>
+      <c r="C1" s="9" t="str">
+        <f>A3</f>
+        <v>PE-LLD</v>
+      </c>
+      <c r="D1" s="9" t="str">
+        <f>A4</f>
+        <v>PE-HD</v>
+      </c>
+      <c r="E1" s="9" t="str">
+        <f>A5</f>
+        <v>PE-MD</v>
+      </c>
+      <c r="F1" s="9" t="str">
+        <f>A6</f>
+        <v>PP</v>
+      </c>
+      <c r="G1" s="9" t="str">
+        <f>A7</f>
+        <v>PS</v>
+      </c>
+      <c r="H1" s="9" t="str">
+        <f>A8</f>
+        <v>PS-E/XPS</v>
+      </c>
+      <c r="I1" s="9" t="str">
+        <f>A9</f>
+        <v>PVC-U</v>
+      </c>
+      <c r="J1" s="9" t="str">
+        <f>A10</f>
+        <v>PVC-P</v>
+      </c>
+      <c r="K1" s="9" t="str">
+        <f>A11</f>
+        <v>ABS</v>
+      </c>
+      <c r="L1" s="9" t="str">
+        <f>A12</f>
+        <v>ASA</v>
+      </c>
+      <c r="M1" s="9" t="str">
+        <f>A13</f>
+        <v>SAN</v>
+      </c>
+      <c r="N1" s="9" t="str">
+        <f>A14</f>
+        <v>PMMA</v>
+      </c>
+      <c r="O1" s="9" t="str">
+        <f>A15</f>
+        <v>PA</v>
+      </c>
+      <c r="P1" s="9" t="str">
+        <f>A16</f>
+        <v>PET</v>
+      </c>
+      <c r="Q1" s="9" t="str">
+        <f>A17</f>
+        <v>POM</v>
+      </c>
+      <c r="R1" s="9" t="str">
+        <f>A18</f>
+        <v>PBT</v>
+      </c>
+      <c r="S1" s="9" t="str">
+        <f>A19</f>
+        <v>PEEK</v>
+      </c>
+      <c r="T1" s="9" t="str">
+        <f>A20</f>
+        <v>PC</v>
+      </c>
+      <c r="U1" s="9" t="str">
+        <f>A21</f>
+        <v>PUR</v>
+      </c>
+      <c r="V1" s="1" t="str">
+        <f>A22</f>
+        <v>Thermoplaste</v>
+      </c>
+      <c r="W1" s="1" t="str">
+        <f>A23</f>
+        <v>Elastomere</v>
+      </c>
+      <c r="X1" s="1" t="str">
+        <f>A24</f>
+        <v>Duromere</v>
+      </c>
+      <c r="Y1" s="1" t="str">
+        <f>A25</f>
+        <v>Aluminium</v>
+      </c>
+      <c r="Z1" s="1" t="str">
+        <f>A26</f>
+        <v>Blei</v>
+      </c>
+      <c r="AA1" s="1" t="str">
+        <f>A27</f>
+        <v>Chrom</v>
+      </c>
+      <c r="AB1" s="1" t="str">
+        <f>A28</f>
+        <v>Eisen</v>
+      </c>
+      <c r="AC1" s="1" t="str">
+        <f>A29</f>
+        <v>Kupfer</v>
+      </c>
+      <c r="AD1" s="1" t="str">
+        <f>A30</f>
+        <v>Magnesium</v>
+      </c>
+      <c r="AE1" s="1" t="str">
+        <f>A31</f>
+        <v>Nickel</v>
+      </c>
+      <c r="AF1" s="1" t="str">
+        <f>A32</f>
+        <v>Stahl</v>
+      </c>
+      <c r="AG1" s="1" t="str">
+        <f>A33</f>
+        <v>Titan</v>
+      </c>
+      <c r="AH1" s="1" t="str">
+        <f>A34</f>
+        <v>Zink</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="str">
+        <f>list_material!A2</f>
+        <v>PE-LD</v>
+      </c>
+      <c r="B2" s="9">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V2" s="9">
+        <v>0</v>
+      </c>
+      <c r="W2" s="9">
+        <v>0</v>
+      </c>
+      <c r="X2" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="str">
+        <f>list_material!A3</f>
+        <v>PE-LLD</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U3" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V3" s="9">
+        <v>0</v>
+      </c>
+      <c r="W3" s="9">
+        <v>0</v>
+      </c>
+      <c r="X3" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="str">
+        <f>list_material!A4</f>
+        <v>PE-HD</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V4" s="9">
+        <v>0</v>
+      </c>
+      <c r="W4" s="9">
+        <v>0</v>
+      </c>
+      <c r="X4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="str">
+        <f>list_material!A5</f>
+        <v>PE-MD</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U5" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V5" s="9">
+        <v>0</v>
+      </c>
+      <c r="W5" s="9">
+        <v>0</v>
+      </c>
+      <c r="X5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="str">
+        <f>list_material!A6</f>
+        <v>PP</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V6" s="9">
+        <v>0</v>
+      </c>
+      <c r="W6" s="9">
+        <v>0</v>
+      </c>
+      <c r="X6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="str">
+        <f>list_material!A7</f>
+        <v>PS</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V7" s="9">
+        <v>0</v>
+      </c>
+      <c r="W7" s="9">
+        <v>0</v>
+      </c>
+      <c r="X7" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="str">
+        <f>list_material!A8</f>
+        <v>PS-E/XPS</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U8" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V8" s="9">
+        <v>0</v>
+      </c>
+      <c r="W8" s="9">
+        <v>0</v>
+      </c>
+      <c r="X8" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="str">
+        <f>list_material!A9</f>
+        <v>PVC-U</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V9" s="9">
+        <v>0</v>
+      </c>
+      <c r="W9" s="9">
+        <v>0</v>
+      </c>
+      <c r="X9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="str">
+        <f>list_material!A10</f>
+        <v>PVC-P</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V10" s="9">
+        <v>0</v>
+      </c>
+      <c r="W10" s="9">
+        <v>0</v>
+      </c>
+      <c r="X10" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="str">
+        <f>list_material!A11</f>
+        <v>ABS</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V11" s="9">
+        <v>0</v>
+      </c>
+      <c r="W11" s="9">
+        <v>0</v>
+      </c>
+      <c r="X11" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="str">
+        <f>list_material!A12</f>
+        <v>ASA</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L12" s="9">
+        <v>0</v>
+      </c>
+      <c r="M12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V12" s="9">
+        <v>0</v>
+      </c>
+      <c r="W12" s="9">
+        <v>0</v>
+      </c>
+      <c r="X12" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="str">
+        <f>list_material!A13</f>
+        <v>SAN</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
+      <c r="N13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V13" s="9">
+        <v>0</v>
+      </c>
+      <c r="W13" s="9">
+        <v>0</v>
+      </c>
+      <c r="X13" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="str">
+        <f>list_material!A14</f>
+        <v>PMMA</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N14" s="9">
+        <v>0</v>
+      </c>
+      <c r="O14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V14" s="9">
+        <v>0</v>
+      </c>
+      <c r="W14" s="9">
+        <v>0</v>
+      </c>
+      <c r="X14" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="str">
+        <f>list_material!A15</f>
+        <v>PA</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O15" s="9">
+        <v>0</v>
+      </c>
+      <c r="P15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V15" s="9">
+        <v>0</v>
+      </c>
+      <c r="W15" s="9">
+        <v>0</v>
+      </c>
+      <c r="X15" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="str">
+        <f>list_material!A16</f>
+        <v>PET</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P16" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V16" s="9">
+        <v>0</v>
+      </c>
+      <c r="W16" s="9">
+        <v>0</v>
+      </c>
+      <c r="X16" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="str">
+        <f>list_material!A17</f>
+        <v>POM</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>0</v>
+      </c>
+      <c r="R17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U17" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V17" s="9">
+        <v>0</v>
+      </c>
+      <c r="W17" s="9">
+        <v>0</v>
+      </c>
+      <c r="X17" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="str">
+        <f>list_material!A18</f>
+        <v>PBT</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R18" s="9">
+        <v>0</v>
+      </c>
+      <c r="S18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U18" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V18" s="9">
+        <v>0</v>
+      </c>
+      <c r="W18" s="9">
+        <v>0</v>
+      </c>
+      <c r="X18" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="str">
+        <f>list_material!A19</f>
+        <v>PEEK</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S19" s="9">
+        <v>0</v>
+      </c>
+      <c r="T19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U19" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V19" s="9">
+        <v>0</v>
+      </c>
+      <c r="W19" s="9">
+        <v>0</v>
+      </c>
+      <c r="X19" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="str">
+        <f>list_material!A20</f>
+        <v>PC</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T20" s="9">
+        <v>0</v>
+      </c>
+      <c r="U20" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="V20" s="9">
+        <v>0</v>
+      </c>
+      <c r="W20" s="9">
+        <v>0</v>
+      </c>
+      <c r="X20" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="str">
+        <f>list_material!A21</f>
+        <v>PUR</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="N21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="O21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="S21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="T21" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="U21" s="9">
+        <v>0</v>
+      </c>
+      <c r="V21" s="9">
+        <v>0</v>
+      </c>
+      <c r="W21" s="9">
+        <v>0</v>
+      </c>
+      <c r="X21" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="str">
+        <f>list_material!A22</f>
+        <v>Thermoplaste</v>
+      </c>
+      <c r="B22" s="9">
+        <v>0</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+      <c r="I22" s="9">
+        <v>0</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0</v>
+      </c>
+      <c r="L22" s="9">
+        <v>0</v>
+      </c>
+      <c r="M22" s="9">
+        <v>0</v>
+      </c>
+      <c r="N22" s="9">
+        <v>0</v>
+      </c>
+      <c r="O22" s="9">
+        <v>0</v>
+      </c>
+      <c r="P22" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="9">
+        <v>0</v>
+      </c>
+      <c r="R22" s="9">
+        <v>0</v>
+      </c>
+      <c r="S22" s="9">
+        <v>0</v>
+      </c>
+      <c r="T22" s="9">
+        <v>0</v>
+      </c>
+      <c r="U22" s="9">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22" s="9">
+        <v>0</v>
+      </c>
+      <c r="X22" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="str">
+        <f>list_material!A23</f>
+        <v>Elastomere</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0</v>
+      </c>
+      <c r="L23" s="9">
+        <v>0</v>
+      </c>
+      <c r="M23" s="9">
+        <v>0</v>
+      </c>
+      <c r="N23" s="9">
+        <v>0</v>
+      </c>
+      <c r="O23" s="9">
+        <v>0</v>
+      </c>
+      <c r="P23" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="9">
+        <v>0</v>
+      </c>
+      <c r="R23" s="9">
+        <v>0</v>
+      </c>
+      <c r="S23" s="9">
+        <v>0</v>
+      </c>
+      <c r="T23" s="9">
+        <v>0</v>
+      </c>
+      <c r="U23" s="9">
+        <v>0</v>
+      </c>
+      <c r="V23" s="9">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="str">
+        <f>list_material!A24</f>
+        <v>Duromere</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0</v>
+      </c>
+      <c r="K24" s="9">
+        <v>0</v>
+      </c>
+      <c r="L24" s="9">
+        <v>0</v>
+      </c>
+      <c r="M24" s="9">
+        <v>0</v>
+      </c>
+      <c r="N24" s="9">
+        <v>0</v>
+      </c>
+      <c r="O24" s="9">
+        <v>0</v>
+      </c>
+      <c r="P24" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>0</v>
+      </c>
+      <c r="R24" s="9">
+        <v>0</v>
+      </c>
+      <c r="S24" s="9">
+        <v>0</v>
+      </c>
+      <c r="T24" s="9">
+        <v>0</v>
+      </c>
+      <c r="U24" s="9">
+        <v>0</v>
+      </c>
+      <c r="V24" s="9">
+        <v>0</v>
+      </c>
+      <c r="W24" s="9">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="str">
+        <f>list_material!A25</f>
+        <v>Aluminium</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0</v>
+      </c>
+      <c r="N25" s="9">
+        <v>0</v>
+      </c>
+      <c r="O25" s="9">
+        <v>0</v>
+      </c>
+      <c r="P25" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="9">
+        <v>0</v>
+      </c>
+      <c r="R25" s="9">
+        <v>0</v>
+      </c>
+      <c r="S25" s="9">
+        <v>0</v>
+      </c>
+      <c r="T25" s="9">
+        <v>0</v>
+      </c>
+      <c r="U25" s="9">
+        <v>0</v>
+      </c>
+      <c r="V25" s="9">
+        <v>0</v>
+      </c>
+      <c r="W25" s="9">
+        <v>0</v>
+      </c>
+      <c r="X25" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="str">
+        <f>list_material!A26</f>
+        <v>Blei</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="9">
+        <v>0</v>
+      </c>
+      <c r="I26" s="9">
+        <v>0</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0</v>
+      </c>
+      <c r="L26" s="9">
+        <v>0</v>
+      </c>
+      <c r="M26" s="9">
+        <v>0</v>
+      </c>
+      <c r="N26" s="9">
+        <v>0</v>
+      </c>
+      <c r="O26" s="9">
+        <v>0</v>
+      </c>
+      <c r="P26" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="9">
+        <v>0</v>
+      </c>
+      <c r="R26" s="9">
+        <v>0</v>
+      </c>
+      <c r="S26" s="9">
+        <v>0</v>
+      </c>
+      <c r="T26" s="9">
+        <v>0</v>
+      </c>
+      <c r="U26" s="9">
+        <v>0</v>
+      </c>
+      <c r="V26" s="9">
+        <v>0</v>
+      </c>
+      <c r="W26" s="9">
+        <v>0</v>
+      </c>
+      <c r="X26" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="str">
+        <f>list_material!A27</f>
+        <v>Chrom</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0</v>
+      </c>
+      <c r="I27" s="9">
+        <v>0</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0</v>
+      </c>
+      <c r="N27" s="9">
+        <v>0</v>
+      </c>
+      <c r="O27" s="9">
+        <v>0</v>
+      </c>
+      <c r="P27" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="9">
+        <v>0</v>
+      </c>
+      <c r="R27" s="9">
+        <v>0</v>
+      </c>
+      <c r="S27" s="9">
+        <v>0</v>
+      </c>
+      <c r="T27" s="9">
+        <v>0</v>
+      </c>
+      <c r="U27" s="9">
+        <v>0</v>
+      </c>
+      <c r="V27" s="9">
+        <v>0</v>
+      </c>
+      <c r="W27" s="9">
+        <v>0</v>
+      </c>
+      <c r="X27" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="str">
+        <f>list_material!A28</f>
+        <v>Eisen</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0</v>
+      </c>
+      <c r="K28" s="9">
+        <v>0</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0</v>
+      </c>
+      <c r="N28" s="9">
+        <v>0</v>
+      </c>
+      <c r="O28" s="9">
+        <v>0</v>
+      </c>
+      <c r="P28" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>0</v>
+      </c>
+      <c r="R28" s="9">
+        <v>0</v>
+      </c>
+      <c r="S28" s="9">
+        <v>0</v>
+      </c>
+      <c r="T28" s="9">
+        <v>0</v>
+      </c>
+      <c r="U28" s="9">
+        <v>0</v>
+      </c>
+      <c r="V28" s="9">
+        <v>0</v>
+      </c>
+      <c r="W28" s="9">
+        <v>0</v>
+      </c>
+      <c r="X28" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="str">
+        <f>list_material!A29</f>
+        <v>Kupfer</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+      <c r="K29" s="9">
+        <v>0</v>
+      </c>
+      <c r="L29" s="9">
+        <v>0</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0</v>
+      </c>
+      <c r="N29" s="9">
+        <v>0</v>
+      </c>
+      <c r="O29" s="9">
+        <v>0</v>
+      </c>
+      <c r="P29" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="9">
+        <v>0</v>
+      </c>
+      <c r="R29" s="9">
+        <v>0</v>
+      </c>
+      <c r="S29" s="9">
+        <v>0</v>
+      </c>
+      <c r="T29" s="9">
+        <v>0</v>
+      </c>
+      <c r="U29" s="9">
+        <v>0</v>
+      </c>
+      <c r="V29" s="9">
+        <v>0</v>
+      </c>
+      <c r="W29" s="9">
+        <v>0</v>
+      </c>
+      <c r="X29" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="str">
+        <f>list_material!A30</f>
+        <v>Magnesium</v>
+      </c>
+      <c r="B30" s="9">
+        <v>0</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
+        <v>0</v>
+      </c>
+      <c r="H30" s="9">
+        <v>0</v>
+      </c>
+      <c r="I30" s="9">
+        <v>0</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0</v>
+      </c>
+      <c r="K30" s="9">
+        <v>0</v>
+      </c>
+      <c r="L30" s="9">
+        <v>0</v>
+      </c>
+      <c r="M30" s="9">
+        <v>0</v>
+      </c>
+      <c r="N30" s="9">
+        <v>0</v>
+      </c>
+      <c r="O30" s="9">
+        <v>0</v>
+      </c>
+      <c r="P30" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="9">
+        <v>0</v>
+      </c>
+      <c r="R30" s="9">
+        <v>0</v>
+      </c>
+      <c r="S30" s="9">
+        <v>0</v>
+      </c>
+      <c r="T30" s="9">
+        <v>0</v>
+      </c>
+      <c r="U30" s="9">
+        <v>0</v>
+      </c>
+      <c r="V30" s="9">
+        <v>0</v>
+      </c>
+      <c r="W30" s="9">
+        <v>0</v>
+      </c>
+      <c r="X30" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="str">
+        <f>list_material!A31</f>
+        <v>Nickel</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9">
+        <v>0</v>
+      </c>
+      <c r="F31" s="9">
+        <v>0</v>
+      </c>
+      <c r="G31" s="9">
+        <v>0</v>
+      </c>
+      <c r="H31" s="9">
+        <v>0</v>
+      </c>
+      <c r="I31" s="9">
+        <v>0</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0</v>
+      </c>
+      <c r="K31" s="9">
+        <v>0</v>
+      </c>
+      <c r="L31" s="9">
+        <v>0</v>
+      </c>
+      <c r="M31" s="9">
+        <v>0</v>
+      </c>
+      <c r="N31" s="9">
+        <v>0</v>
+      </c>
+      <c r="O31" s="9">
+        <v>0</v>
+      </c>
+      <c r="P31" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="9">
+        <v>0</v>
+      </c>
+      <c r="R31" s="9">
+        <v>0</v>
+      </c>
+      <c r="S31" s="9">
+        <v>0</v>
+      </c>
+      <c r="T31" s="9">
+        <v>0</v>
+      </c>
+      <c r="U31" s="9">
+        <v>0</v>
+      </c>
+      <c r="V31" s="9">
+        <v>0</v>
+      </c>
+      <c r="W31" s="9">
+        <v>0</v>
+      </c>
+      <c r="X31" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="str">
+        <f>list_material!A32</f>
+        <v>Stahl</v>
+      </c>
+      <c r="B32" s="9">
+        <v>0</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0</v>
+      </c>
+      <c r="F32" s="9">
+        <v>0</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0</v>
+      </c>
+      <c r="H32" s="9">
+        <v>0</v>
+      </c>
+      <c r="I32" s="9">
+        <v>0</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0</v>
+      </c>
+      <c r="K32" s="9">
+        <v>0</v>
+      </c>
+      <c r="L32" s="9">
+        <v>0</v>
+      </c>
+      <c r="M32" s="9">
+        <v>0</v>
+      </c>
+      <c r="N32" s="9">
+        <v>0</v>
+      </c>
+      <c r="O32" s="9">
+        <v>0</v>
+      </c>
+      <c r="P32" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="9">
+        <v>0</v>
+      </c>
+      <c r="R32" s="9">
+        <v>0</v>
+      </c>
+      <c r="S32" s="9">
+        <v>0</v>
+      </c>
+      <c r="T32" s="9">
+        <v>0</v>
+      </c>
+      <c r="U32" s="9">
+        <v>0</v>
+      </c>
+      <c r="V32" s="9">
+        <v>0</v>
+      </c>
+      <c r="W32" s="9">
+        <v>0</v>
+      </c>
+      <c r="X32" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="str">
+        <f>list_material!A33</f>
+        <v>Titan</v>
+      </c>
+      <c r="B33" s="9">
+        <v>0</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0</v>
+      </c>
+      <c r="L33" s="9">
+        <v>0</v>
+      </c>
+      <c r="M33" s="9">
+        <v>0</v>
+      </c>
+      <c r="N33" s="9">
+        <v>0</v>
+      </c>
+      <c r="O33" s="9">
+        <v>0</v>
+      </c>
+      <c r="P33" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="9">
+        <v>0</v>
+      </c>
+      <c r="R33" s="9">
+        <v>0</v>
+      </c>
+      <c r="S33" s="9">
+        <v>0</v>
+      </c>
+      <c r="T33" s="9">
+        <v>0</v>
+      </c>
+      <c r="U33" s="9">
+        <v>0</v>
+      </c>
+      <c r="V33" s="9">
+        <v>0</v>
+      </c>
+      <c r="W33" s="9">
+        <v>0</v>
+      </c>
+      <c r="X33" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="str">
+        <f>list_material!A34</f>
+        <v>Zink</v>
+      </c>
+      <c r="B34" s="9">
+        <v>0</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9">
+        <v>0</v>
+      </c>
+      <c r="F34" s="9">
+        <v>0</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0</v>
+      </c>
+      <c r="H34" s="9">
+        <v>0</v>
+      </c>
+      <c r="I34" s="9">
+        <v>0</v>
+      </c>
+      <c r="J34" s="9">
+        <v>0</v>
+      </c>
+      <c r="K34" s="9">
+        <v>0</v>
+      </c>
+      <c r="L34" s="9">
+        <v>0</v>
+      </c>
+      <c r="M34" s="9">
+        <v>0</v>
+      </c>
+      <c r="N34" s="9">
+        <v>0</v>
+      </c>
+      <c r="O34" s="9">
+        <v>0</v>
+      </c>
+      <c r="P34" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="9">
+        <v>0</v>
+      </c>
+      <c r="R34" s="9">
+        <v>0</v>
+      </c>
+      <c r="S34" s="9">
+        <v>0</v>
+      </c>
+      <c r="T34" s="9">
+        <v>0</v>
+      </c>
+      <c r="U34" s="9">
+        <v>0</v>
+      </c>
+      <c r="V34" s="9">
+        <v>0</v>
+      </c>
+      <c r="W34" s="9">
+        <v>0</v>
+      </c>
+      <c r="X34" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FB39F2-18C7-4C89-AECD-A2AD62B3166C}">
   <dimension ref="A1:F106"/>
   <sheetViews>

</xml_diff>